<commit_message>
feat(NDF_Generator): Environment verifications et optional installations
</commit_message>
<xml_diff>
--- a/A_MODIFIER/data.xlsx
+++ b/A_MODIFIER/data.xlsx
@@ -8,7 +8,7 @@
   <sheets>
     <sheet name="Tableau de bord" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Bénéficiaires" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Options" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Options" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Bénéficiaires!$A$1:$E$2</definedName>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Quantité</t>
   </si>
@@ -42,7 +42,7 @@
     <t>Données</t>
   </si>
   <si>
-    <t>test</t>
+    <t xml:space="preserve">Ballons de basket</t>
   </si>
   <si>
     <t xml:space="preserve">Adresse de l'association (partie 1)</t>
@@ -51,22 +51,34 @@
     <t xml:space="preserve">2 rue Charles Camichel</t>
   </si>
   <si>
+    <t xml:space="preserve">Panier de basket</t>
+  </si>
+  <si>
     <t xml:space="preserve">Adresse de l'association (partie 2)</t>
   </si>
   <si>
     <t xml:space="preserve">31071 Toulouse CEDEX 7</t>
   </si>
   <si>
+    <t xml:space="preserve">Paire de chaussure</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fait à</t>
   </si>
   <si>
     <t>Toulouse</t>
   </si>
   <si>
+    <t>Maillots</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nom de l'association</t>
   </si>
   <si>
     <t>Wallstreet</t>
+  </si>
+  <si>
+    <t>Short</t>
   </si>
   <si>
     <t xml:space="preserve">Email de l'association</t>
@@ -214,11 +226,14 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -756,16 +771,16 @@
     </row>
     <row r="2" ht="14.25">
       <c r="A2">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D2">
-        <v>12</v>
+        <v>240</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>7</v>
@@ -775,51 +790,83 @@
       </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4">
+        <v>325</v>
+      </c>
+      <c r="D3" s="4">
+        <v>325</v>
+      </c>
       <c r="F3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" s="4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="4">
+        <v>150</v>
+      </c>
+      <c r="D4" s="4">
+        <v>150</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5" s="4">
+        <v>25</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" ht="14.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="F4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" ht="14.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="D5" s="4">
+        <v>250</v>
+      </c>
       <c r="F5" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="A6" s="4">
+        <v>25</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="4">
+        <v>15</v>
+      </c>
+      <c r="D6" s="4">
+        <v>375</v>
+      </c>
       <c r="F6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" ht="14.25">
@@ -828,10 +875,10 @@
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="F7" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" ht="14.25">
@@ -840,61 +887,61 @@
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="F8" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" ht="14.25">
       <c r="F9" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" ht="14.25">
       <c r="F10" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G10" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" ht="14.25">
       <c r="F11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="12" ht="14.25">
       <c r="F12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="13" ht="14.25">
       <c r="F13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G13" s="6"/>
+        <v>33</v>
+      </c>
+      <c r="G13" s="7"/>
     </row>
     <row r="14" ht="14.25">
       <c r="F14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" s="6">
+        <v>34</v>
+      </c>
+      <c r="G14" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="15" ht="14.25">
       <c r="F15" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="G15" s="3" t="str">
         <f>_xlfn.XLOOKUP(G11,Bénéficiaires!A:A,Bénéficiaires!B:B,"Adresse non-renseignée")</f>
@@ -903,7 +950,7 @@
     </row>
     <row r="16" ht="14.25">
       <c r="F16" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G16" s="3" t="str">
         <f>_xlfn.XLOOKUP(G11,Bénéficiaires!A:A,Bénéficiaires!C:C,"Adresse non-renseignée")</f>
@@ -912,7 +959,7 @@
     </row>
     <row r="17" ht="14.25">
       <c r="F17" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G17" s="3" t="str">
         <f>_xlfn.XLOOKUP(G11,Bénéficiaires!A:A,Bénéficiaires!D:D,"Téléphone non-renseigné")</f>
@@ -921,7 +968,7 @@
     </row>
     <row r="18" ht="14.25">
       <c r="F18" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G18" t="str">
         <f>IF(G12="Virement bancaire",_xlfn.XLOOKUP(G11,Bénéficiaires!A:A,Bénéficiaires!E:E,"IBAN non-renseigné"),"")</f>
@@ -964,36 +1011,36 @@
   <sheetData>
     <row r="1" ht="14.25">
       <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" ht="14.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1023,22 +1070,22 @@
   <sheetData>
     <row r="1" ht="14.25">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" ht="14.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add manual input for final_price, improve README.md
</commit_message>
<xml_diff>
--- a/A_MODIFIER/data.xlsx
+++ b/A_MODIFIER/data.xlsx
@@ -1,42 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hourl\HOME\expense-report-creator\A_MODIFIER\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{575A7C31-BEEA-4EBF-A999-C366564DBD22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Tableau de bord" sheetId="1" r:id="rId1"/>
-    <sheet name="Bénéficiaires" sheetId="2" r:id="rId2"/>
+    <sheet name="Tableau de bord" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Bénéficiaires" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Options" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Bénéficiaires!$A$1:$E$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Bénéficiaires!$A$1:$E$2</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}"/>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Quantité</t>
   </si>
@@ -44,10 +30,10 @@
     <t>Référence</t>
   </si>
   <si>
-    <t>Prix unitaire</t>
-  </si>
-  <si>
-    <t>Prix total</t>
+    <t xml:space="preserve">Prix unitaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prix total</t>
   </si>
   <si>
     <t>Champs</t>
@@ -56,31 +42,37 @@
     <t>Données</t>
   </si>
   <si>
-    <t>Adresse de l'association (partie 1)</t>
-  </si>
-  <si>
-    <t>2 rue Charles Camichel</t>
-  </si>
-  <si>
-    <t>Panier de basket</t>
-  </si>
-  <si>
-    <t>Adresse de l'association (partie 2)</t>
-  </si>
-  <si>
-    <t>31071 Toulouse CEDEX 7</t>
-  </si>
-  <si>
-    <t>Paire de chaussure</t>
-  </si>
-  <si>
-    <t>Fait à</t>
+    <t xml:space="preserve">Ballon de basket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adresse de l'association (partie 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 rue Charles Camichel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panier de basket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adresse de l'association (partie 2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31071 Toulouse CEDEX 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paire de chaussure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fait à</t>
   </si>
   <si>
     <t>Toulouse</t>
   </si>
   <si>
-    <t>Nom de l'association</t>
+    <t>Maillot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nom de l'association</t>
   </si>
   <si>
     <t>Wallstreet</t>
@@ -89,7 +81,7 @@
     <t>Short</t>
   </si>
   <si>
-    <t>Email de l'association</t>
+    <t xml:space="preserve">Email de l'association</t>
   </si>
   <si>
     <t>jordan.belfort@gmail.com</t>
@@ -104,112 +96,109 @@
     <t>Trésorier</t>
   </si>
   <si>
-    <t>Jordan Belfort</t>
-  </si>
-  <si>
-    <t>Nom du fichier logo (vide si pas)</t>
+    <t xml:space="preserve">Jordan Belfort</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nom du fichier logo (vide si pas)</t>
   </si>
   <si>
     <t>logo.png</t>
   </si>
   <si>
-    <t>Nom du fichier signature (vide si pas)</t>
+    <t xml:space="preserve">Nom du fichier signature (vide si pas)</t>
   </si>
   <si>
     <t>signature.png</t>
   </si>
   <si>
-    <t>Bénéficiaire (à remplir sur la feuille suivante)</t>
-  </si>
-  <si>
-    <t>Michael Jordan</t>
-  </si>
-  <si>
-    <t>Mode de remboursement</t>
-  </si>
-  <si>
-    <t>Virement bancaire</t>
-  </si>
-  <si>
-    <t>Noms pièces jointes (séparées par une virgule)</t>
-  </si>
-  <si>
-    <t>Numéro de la note de frais</t>
-  </si>
-  <si>
-    <t>Adresse (partie 1)</t>
-  </si>
-  <si>
-    <t>Adresse (partie 2)</t>
+    <t xml:space="preserve">Bénéficiaire (à remplir sur la feuille suivante)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michael Jordan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mode de remboursement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virement bancaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noms pièces jointes (séparées par une virgule)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numéro de la note de frais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remboursement total (auto si vide)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adresse (partie 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adresse (partie 2)</t>
   </si>
   <si>
     <t>Téléphone</t>
   </si>
   <si>
-    <t>IBAN (remplissage auto à partir du bénéficiaire)</t>
-  </si>
-  <si>
-    <t>Prénom Nom</t>
-  </si>
-  <si>
-    <t>Téléphone (ou email)</t>
+    <t xml:space="preserve">IBAN (remplissage auto à partir du bénéficiaire)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prénom Nom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Téléphone (ou email)</t>
   </si>
   <si>
     <t>IBAN</t>
   </si>
   <si>
-    <t>200 rue du Basket</t>
-  </si>
-  <si>
-    <t>31000 Toulouse</t>
-  </si>
-  <si>
-    <t>06 69 69 69 69</t>
-  </si>
-  <si>
-    <t>FR76 0000 0000 5700 0408 9597 000</t>
+    <t xml:space="preserve">200 rue du Basket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31000 Toulouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06 69 69 69 69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FR76 0000 0000 5700 0408 9597 000</t>
   </si>
   <si>
     <t>Espèce</t>
   </si>
   <si>
-    <t>Application de transfert</t>
-  </si>
-  <si>
-    <t>Ballon de basket</t>
-  </si>
-  <si>
-    <t>Maillot</t>
+    <t xml:space="preserve">Application de transfert</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4">
     <font>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <i/>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color theme="10"/>
       <name val="Calibri"/>
     </font>
@@ -230,22 +219,22 @@
   </fills>
   <borders count="1">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -263,8 +252,291 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Angsana New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="New Office">
       <a:dk1>
@@ -455,29 +727,27 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
-    <col min="3" max="4" width="17.140625" customWidth="1"/>
-    <col min="5" max="5" width="4.85546875" customWidth="1"/>
-    <col min="6" max="6" width="42.85546875" customWidth="1"/>
-    <col min="7" max="7" width="34.5703125" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="17.140625"/>
+    <col customWidth="1" min="2" max="2" width="20.28515625"/>
+    <col customWidth="1" min="3" max="4" width="17.140625"/>
+    <col customWidth="1" min="5" max="5" width="4.85546875"/>
+    <col customWidth="1" min="6" max="6" width="42.85546875"/>
+    <col customWidth="1" min="7" max="7" width="34.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -497,12 +767,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2">
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>20</v>
@@ -511,18 +781,18 @@
         <v>240</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <v>325</v>
@@ -531,18 +801,18 @@
         <v>325</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>150</v>
@@ -551,18 +821,18 @@
         <v>150</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5">
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <v>10</v>
@@ -571,18 +841,18 @@
         <v>250</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6">
         <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C6">
         <v>15</v>
@@ -591,229 +861,233 @@
         <v>375</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="F7" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="F8" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="F9" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="F10" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="F11" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12">
       <c r="F12" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13">
       <c r="F13" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14">
       <c r="F14" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G14" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" t="str">
+    <row r="15">
+      <c r="F15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16">
+      <c r="F16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" t="str">
         <f>_xlfn.XLOOKUP(G11,Bénéficiaires!A:A,Bénéficiaires!B:B,"Adresse non-renseignée")</f>
-        <v>200 rue du Basket</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F16" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G16" t="str">
+        <v xml:space="preserve">200 rue du Basket</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="F17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" t="str">
         <f>_xlfn.XLOOKUP(G11,Bénéficiaires!A:A,Bénéficiaires!C:C,"Adresse non-renseignée")</f>
-        <v>31000 Toulouse</v>
-      </c>
-    </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F17" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G17" t="str">
+        <v xml:space="preserve">31000 Toulouse</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="F18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" t="str">
         <f>_xlfn.XLOOKUP(G11,Bénéficiaires!A:A,Bénéficiaires!D:D,"Téléphone non-renseigné")</f>
-        <v>06 69 69 69 69</v>
-      </c>
-    </row>
-    <row r="18" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G18" t="str">
+        <v xml:space="preserve">06 69 69 69 69</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="F19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" t="str">
         <f>IF(G12="Virement bancaire",_xlfn.XLOOKUP(G11,Bénéficiaires!A:A,Bénéficiaires!E:E,"IBAN non-renseigné"),"")</f>
-        <v>FR76 0000 0000 5700 0408 9597 000</v>
+        <v xml:space="preserve">FR76 0000 0000 5700 0408 9597 000</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2" disablePrompts="0">
+    <dataValidation sqref="G11" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+      <formula1>Bénéficiaires!$A$2:$A$1000</formula1>
+    </dataValidation>
+    <dataValidation sqref="G12" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+      <formula1>Options!$A$2:$A$4</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink r:id="rId1" ref="G6"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
-          <x14:formula1>
-            <xm:f>Bénéficiaires!$A$2:$A$1000</xm:f>
-          </x14:formula1>
-          <xm:sqref>G11</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
-          <x14:formula1>
-            <xm:f>Options!$A$2:$A$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>G12</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="0" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="39" customWidth="1"/>
-    <col min="5" max="5" width="36.28515625" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="24.140625"/>
+    <col customWidth="1" min="2" max="3" width="23.140625"/>
+    <col customWidth="1" min="4" max="4" width="39"/>
+    <col customWidth="1" min="5" max="5" width="36.28515625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E2" xr:uid="{00000000-0009-0000-0000-000001000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
+  <autoFilter ref="A1:E2">
+    <sortState ref="A2:E2">
       <sortCondition ref="A1:A2"/>
     </sortState>
   </autoFilter>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:A4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="24.28515625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>